<commit_message>
add pole wypt (orgin = 0)
</commit_message>
<xml_diff>
--- a/Data/receivers_GPS.xlsx
+++ b/Data/receivers_GPS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fiudit-my.sharepoint.com/personal/rsantosc_fiu_edu/Documents/R_Git/Shrimp_YAPS_Test/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{2E7FF655-FBD9-4F08-B891-3A3AF916E6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAC8F658-8269-48D4-A703-541D06814726}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{2E7FF655-FBD9-4F08-B891-3A3AF916E6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74B96892-8EF1-4A4F-BFBF-E625A18E38D2}"/>
   <bookViews>
-    <workbookView xWindow="-23910" yWindow="0" windowWidth="12000" windowHeight="12900" xr2:uid="{704F37CA-3A0E-4CA4-A497-9A1DF572C560}"/>
+    <workbookView xWindow="-24000" yWindow="0" windowWidth="12000" windowHeight="12900" xr2:uid="{704F37CA-3A0E-4CA4-A497-9A1DF572C560}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -471,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0520C27B-09DD-4851-95D8-8196724963A5}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -662,6 +662,47 @@
         <v>202231.04111578999</v>
       </c>
     </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>36</v>
+      </c>
+      <c r="G5">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1">
+        <v>18.321189</v>
+      </c>
+      <c r="I5" s="1">
+        <v>-65.816972000000007</v>
+      </c>
+      <c r="J5" s="1">
+        <v>18.321231999999998</v>
+      </c>
+      <c r="K5" s="1">
+        <v>-65.816973000000004</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2028023.504987</v>
+      </c>
+      <c r="M5" s="1">
+        <v>202235.59276199999</v>
+      </c>
+      <c r="N5" s="1">
+        <v>2028028.2687830001</v>
+      </c>
+      <c r="O5" s="1">
+        <v>202235.56064800001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>